<commit_message>
after finalizing DABOM results, re-ran the prep data for 2021
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/2021_Steelhead Data.xlsx
+++ b/analysis/data/raw_data/2021_Steelhead Data.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hughemsh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/kevin_see_dfw_wa_gov/Documents/Documents/Git/MyProjects/UCSthdReddObsErr/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A910B6C-E1B7-43D8-890F-5C6CE38FB0D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{8A910B6C-E1B7-43D8-890F-5C6CE38FB0D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DC2D758-0F82-4799-96ED-A4EADA845053}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7214952A-1BD3-4C9C-A7BA-38E60CEF622C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{7214952A-1BD3-4C9C-A7BA-38E60CEF622C}"/>
   </bookViews>
   <sheets>
     <sheet name="Census 2021" sheetId="1" r:id="rId1"/>
     <sheet name="Tributaries 2021" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Census 2021'!$A$1:$P$71</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -753,15 +756,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04D094B6-8BD2-4BDC-B0AB-897414B62CF9}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:P71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T18" sqref="T18"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="32.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -811,7 +815,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -859,7 +863,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -907,7 +911,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -955,7 +959,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1003,7 +1007,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1051,7 +1055,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1099,7 +1103,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1147,7 +1151,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1195,7 +1199,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1243,7 +1247,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1291,7 +1295,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1339,7 +1343,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1387,7 +1391,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1435,7 +1439,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1483,7 +1487,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1531,7 +1535,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1579,7 +1583,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1627,7 +1631,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1675,7 +1679,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1723,7 +1727,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1771,7 +1775,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1819,7 +1823,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1867,7 +1871,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1915,7 +1919,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1963,7 +1967,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2011,7 +2015,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2059,7 +2063,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2107,7 +2111,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2155,7 +2159,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2203,7 +2207,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2251,7 +2255,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2299,7 +2303,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2347,7 +2351,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2395,7 +2399,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2443,7 +2447,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2491,7 +2495,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2539,7 +2543,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2587,7 +2591,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2635,7 +2639,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2683,7 +2687,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2731,7 +2735,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2779,7 +2783,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2827,7 +2831,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2875,7 +2879,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2923,7 +2927,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2971,7 +2975,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -3019,7 +3023,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -3067,7 +3071,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -3115,7 +3119,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -3163,7 +3167,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -3211,7 +3215,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -3259,7 +3263,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -3307,7 +3311,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -3355,7 +3359,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -3403,7 +3407,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -3451,7 +3455,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -3499,7 +3503,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -3547,7 +3551,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -3595,7 +3599,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -3643,7 +3647,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -3691,7 +3695,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -3739,7 +3743,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -3787,7 +3791,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -3835,7 +3839,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -3883,7 +3887,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -3931,7 +3935,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -3979,7 +3983,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -4027,7 +4031,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -4075,7 +4079,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -4123,7 +4127,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -4172,6 +4176,18 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:P71" xr:uid="{7277747A-2E56-49D6-95F4-291969B8C6AF}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="W9"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Y"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4185,9 +4201,9 @@
       <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:17" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="32.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4240,7 +4256,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>71</v>
       </c>
@@ -4283,7 +4299,7 @@
       <c r="P2" s="15"/>
       <c r="Q2" s="15"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>72</v>
       </c>
@@ -4326,7 +4342,7 @@
       <c r="P3" s="15"/>
       <c r="Q3" s="15"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>73</v>
       </c>
@@ -4369,7 +4385,7 @@
       <c r="P4" s="15"/>
       <c r="Q4" s="15"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>74</v>
       </c>
@@ -4412,7 +4428,7 @@
       <c r="P5" s="15"/>
       <c r="Q5" s="15"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>75</v>
       </c>
@@ -4455,7 +4471,7 @@
       <c r="P6" s="15"/>
       <c r="Q6" s="15"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>76</v>
       </c>
@@ -4498,7 +4514,7 @@
       <c r="P7" s="15"/>
       <c r="Q7" s="15"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>77</v>
       </c>
@@ -4541,7 +4557,7 @@
       <c r="P8" s="15"/>
       <c r="Q8" s="15"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>78</v>
       </c>
@@ -4584,7 +4600,7 @@
       <c r="P9" s="15"/>
       <c r="Q9" s="15"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>79</v>
       </c>
@@ -4627,7 +4643,7 @@
       <c r="P10" s="15"/>
       <c r="Q10" s="15"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>80</v>
       </c>
@@ -4670,7 +4686,7 @@
       <c r="P11" s="15"/>
       <c r="Q11" s="15"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>81</v>
       </c>
@@ -4713,7 +4729,7 @@
       <c r="P12" s="15"/>
       <c r="Q12" s="15"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>82</v>
       </c>
@@ -4756,7 +4772,7 @@
       <c r="P13" s="15"/>
       <c r="Q13" s="15"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>83</v>
       </c>
@@ -4799,7 +4815,7 @@
       <c r="P14" s="15"/>
       <c r="Q14" s="15"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>84</v>
       </c>
@@ -4842,7 +4858,7 @@
       <c r="P15" s="15"/>
       <c r="Q15" s="15"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>85</v>
       </c>
@@ -4885,7 +4901,7 @@
       <c r="P16" s="15"/>
       <c r="Q16" s="15"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>86</v>
       </c>
@@ -4928,7 +4944,7 @@
       <c r="P17" s="15"/>
       <c r="Q17" s="15"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>87</v>
       </c>
@@ -4971,7 +4987,7 @@
       <c r="P18" s="15"/>
       <c r="Q18" s="15"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>88</v>
       </c>
@@ -5014,7 +5030,7 @@
       <c r="P19" s="15"/>
       <c r="Q19" s="15"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>89</v>
       </c>
@@ -5057,7 +5073,7 @@
       <c r="P20" s="15"/>
       <c r="Q20" s="15"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>90</v>
       </c>
@@ -5100,7 +5116,7 @@
       <c r="P21" s="15"/>
       <c r="Q21" s="15"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>91</v>
       </c>
@@ -5143,7 +5159,7 @@
       <c r="P22" s="15"/>
       <c r="Q22" s="15"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>92</v>
       </c>
@@ -5186,7 +5202,7 @@
       <c r="P23" s="15"/>
       <c r="Q23" s="15"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>93</v>
       </c>
@@ -5229,7 +5245,7 @@
       <c r="P24" s="15"/>
       <c r="Q24" s="15"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>94</v>
       </c>
@@ -5272,7 +5288,7 @@
       <c r="P25" s="15"/>
       <c r="Q25" s="15"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>95</v>
       </c>
@@ -5315,7 +5331,7 @@
       <c r="P26" s="15"/>
       <c r="Q26" s="15"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>96</v>
       </c>
@@ -5358,7 +5374,7 @@
       <c r="P27" s="15"/>
       <c r="Q27" s="15"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>97</v>
       </c>
@@ -5401,7 +5417,7 @@
       <c r="P28" s="15"/>
       <c r="Q28" s="15"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>98</v>
       </c>
@@ -5444,7 +5460,7 @@
       <c r="P29" s="15"/>
       <c r="Q29" s="15"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>99</v>
       </c>
@@ -5487,7 +5503,7 @@
       <c r="P30" s="15"/>
       <c r="Q30" s="15"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>100</v>
       </c>
@@ -5530,7 +5546,7 @@
       <c r="P31" s="15"/>
       <c r="Q31" s="15"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>101</v>
       </c>
@@ -5573,7 +5589,7 @@
       <c r="P32" s="15"/>
       <c r="Q32" s="15"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>102</v>
       </c>
@@ -5616,7 +5632,7 @@
       <c r="P33" s="15"/>
       <c r="Q33" s="15"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>103</v>
       </c>
@@ -5659,7 +5675,7 @@
       <c r="P34" s="15"/>
       <c r="Q34" s="15"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>104</v>
       </c>
@@ -5702,7 +5718,7 @@
       <c r="P35" s="15"/>
       <c r="Q35" s="15"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>105</v>
       </c>
@@ -5745,7 +5761,7 @@
       <c r="P36" s="15"/>
       <c r="Q36" s="15"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>106</v>
       </c>
@@ -5788,7 +5804,7 @@
       <c r="P37" s="15"/>
       <c r="Q37" s="15"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>107</v>
       </c>

</xml_diff>

<commit_message>
added a script for saving data from all years to an MS Teams site in a consistent format
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/2021_Steelhead Data.xlsx
+++ b/analysis/data/raw_data/2021_Steelhead Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/kevin_see_dfw_wa_gov/Documents/Documents/Git/MyProjects/UCSthdReddObsErr/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{8A910B6C-E1B7-43D8-890F-5C6CE38FB0D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DC2D758-0F82-4799-96ED-A4EADA845053}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{8A910B6C-E1B7-43D8-890F-5C6CE38FB0D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E22F665-1EC9-4C3B-86E8-FC659B4C2080}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{7214952A-1BD3-4C9C-A7BA-38E60CEF622C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{7214952A-1BD3-4C9C-A7BA-38E60CEF622C}"/>
   </bookViews>
   <sheets>
     <sheet name="Census 2021" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Census 2021'!$A$1:$P$71</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateCount="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -759,13 +759,13 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="32.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -815,7 +815,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -863,7 +863,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -911,7 +911,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -959,7 +959,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2591,7 +2591,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -3167,7 +3167,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -3215,7 +3215,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -3407,7 +3407,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -3455,7 +3455,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -3647,7 +3647,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -3695,7 +3695,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -3743,7 +3743,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -3791,7 +3791,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -3887,7 +3887,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -3935,7 +3935,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -4031,7 +4031,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -4079,7 +4079,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -4127,7 +4127,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -4177,11 +4177,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:P71" xr:uid="{7277747A-2E56-49D6-95F4-291969B8C6AF}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="W9"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="3">
       <filters>
         <filter val="Y"/>
@@ -4201,9 +4196,9 @@
       <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" ht="32.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4256,7 +4251,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>71</v>
       </c>
@@ -4299,7 +4294,7 @@
       <c r="P2" s="15"/>
       <c r="Q2" s="15"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>72</v>
       </c>
@@ -4342,7 +4337,7 @@
       <c r="P3" s="15"/>
       <c r="Q3" s="15"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>73</v>
       </c>
@@ -4385,7 +4380,7 @@
       <c r="P4" s="15"/>
       <c r="Q4" s="15"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>74</v>
       </c>
@@ -4428,7 +4423,7 @@
       <c r="P5" s="15"/>
       <c r="Q5" s="15"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>75</v>
       </c>
@@ -4471,7 +4466,7 @@
       <c r="P6" s="15"/>
       <c r="Q6" s="15"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>76</v>
       </c>
@@ -4514,7 +4509,7 @@
       <c r="P7" s="15"/>
       <c r="Q7" s="15"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>77</v>
       </c>
@@ -4557,7 +4552,7 @@
       <c r="P8" s="15"/>
       <c r="Q8" s="15"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>78</v>
       </c>
@@ -4600,7 +4595,7 @@
       <c r="P9" s="15"/>
       <c r="Q9" s="15"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>79</v>
       </c>
@@ -4643,7 +4638,7 @@
       <c r="P10" s="15"/>
       <c r="Q10" s="15"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>80</v>
       </c>
@@ -4686,7 +4681,7 @@
       <c r="P11" s="15"/>
       <c r="Q11" s="15"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>81</v>
       </c>
@@ -4729,7 +4724,7 @@
       <c r="P12" s="15"/>
       <c r="Q12" s="15"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>82</v>
       </c>
@@ -4772,7 +4767,7 @@
       <c r="P13" s="15"/>
       <c r="Q13" s="15"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>83</v>
       </c>
@@ -4815,7 +4810,7 @@
       <c r="P14" s="15"/>
       <c r="Q14" s="15"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>84</v>
       </c>
@@ -4858,7 +4853,7 @@
       <c r="P15" s="15"/>
       <c r="Q15" s="15"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>85</v>
       </c>
@@ -4901,7 +4896,7 @@
       <c r="P16" s="15"/>
       <c r="Q16" s="15"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>86</v>
       </c>
@@ -4944,7 +4939,7 @@
       <c r="P17" s="15"/>
       <c r="Q17" s="15"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>87</v>
       </c>
@@ -4987,7 +4982,7 @@
       <c r="P18" s="15"/>
       <c r="Q18" s="15"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>88</v>
       </c>
@@ -5030,7 +5025,7 @@
       <c r="P19" s="15"/>
       <c r="Q19" s="15"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>89</v>
       </c>
@@ -5073,7 +5068,7 @@
       <c r="P20" s="15"/>
       <c r="Q20" s="15"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>90</v>
       </c>
@@ -5116,7 +5111,7 @@
       <c r="P21" s="15"/>
       <c r="Q21" s="15"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>91</v>
       </c>
@@ -5159,7 +5154,7 @@
       <c r="P22" s="15"/>
       <c r="Q22" s="15"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>92</v>
       </c>
@@ -5202,7 +5197,7 @@
       <c r="P23" s="15"/>
       <c r="Q23" s="15"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>93</v>
       </c>
@@ -5245,7 +5240,7 @@
       <c r="P24" s="15"/>
       <c r="Q24" s="15"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>94</v>
       </c>
@@ -5288,7 +5283,7 @@
       <c r="P25" s="15"/>
       <c r="Q25" s="15"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>95</v>
       </c>
@@ -5331,7 +5326,7 @@
       <c r="P26" s="15"/>
       <c r="Q26" s="15"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>96</v>
       </c>
@@ -5374,7 +5369,7 @@
       <c r="P27" s="15"/>
       <c r="Q27" s="15"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>97</v>
       </c>
@@ -5417,7 +5412,7 @@
       <c r="P28" s="15"/>
       <c r="Q28" s="15"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>98</v>
       </c>
@@ -5460,7 +5455,7 @@
       <c r="P29" s="15"/>
       <c r="Q29" s="15"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>99</v>
       </c>
@@ -5503,7 +5498,7 @@
       <c r="P30" s="15"/>
       <c r="Q30" s="15"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>100</v>
       </c>
@@ -5546,7 +5541,7 @@
       <c r="P31" s="15"/>
       <c r="Q31" s="15"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>101</v>
       </c>
@@ -5589,7 +5584,7 @@
       <c r="P32" s="15"/>
       <c r="Q32" s="15"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>102</v>
       </c>
@@ -5632,7 +5627,7 @@
       <c r="P33" s="15"/>
       <c r="Q33" s="15"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>103</v>
       </c>
@@ -5675,7 +5670,7 @@
       <c r="P34" s="15"/>
       <c r="Q34" s="15"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>104</v>
       </c>
@@ -5718,7 +5713,7 @@
       <c r="P35" s="15"/>
       <c r="Q35" s="15"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>105</v>
       </c>
@@ -5761,7 +5756,7 @@
       <c r="P36" s="15"/>
       <c r="Q36" s="15"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>106</v>
       </c>
@@ -5804,7 +5799,7 @@
       <c r="P37" s="15"/>
       <c r="Q37" s="15"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>107</v>
       </c>

</xml_diff>